<commit_message>
changes to sample excel file
</commit_message>
<xml_diff>
--- a/excel_file.xlsx
+++ b/excel_file.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24923"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B379B578-DEB6-4EBA-8222-42B283458FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDC9BC2C-2A12-4BB8-BB9B-087329B6E234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="198">
   <si>
     <t>Subject</t>
   </si>
@@ -55,7 +55,7 @@
     <t>Private</t>
   </si>
   <si>
-    <t>hey 1</t>
+    <t>Subject 1</t>
   </si>
   <si>
     <t>01/21/22</t>
@@ -64,40 +64,46 @@
     <t>2:00</t>
   </si>
   <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Description 1</t>
+  </si>
+  <si>
+    <t>Location 1</t>
+  </si>
+  <si>
     <t>FALSE</t>
   </si>
   <si>
-    <t>AHOY 1</t>
-  </si>
-  <si>
-    <t>Brazil 1</t>
-  </si>
-  <si>
-    <t>hey 2</t>
+    <t>Subject 2</t>
   </si>
   <si>
     <t>3:00</t>
   </si>
   <si>
-    <t>AHOY 2</t>
-  </si>
-  <si>
-    <t>Brazil 2</t>
-  </si>
-  <si>
-    <t>hey 3</t>
+    <t>Description 2</t>
+  </si>
+  <si>
+    <t>Location 2</t>
+  </si>
+  <si>
+    <t>Subject 3</t>
   </si>
   <si>
     <t>4:00</t>
   </si>
   <si>
-    <t>AHOY 3</t>
-  </si>
-  <si>
-    <t>Brazil 3</t>
-  </si>
-  <si>
-    <t>hey 4</t>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Description 3</t>
+  </si>
+  <si>
+    <t>Location 3</t>
+  </si>
+  <si>
+    <t>Subject 4</t>
   </si>
   <si>
     <t>01/24/22</t>
@@ -106,25 +112,25 @@
     <t>5:00</t>
   </si>
   <si>
-    <t>AHOY 4</t>
-  </si>
-  <si>
-    <t>Brazil 4</t>
-  </si>
-  <si>
-    <t>hey 5</t>
+    <t>Description 4</t>
+  </si>
+  <si>
+    <t>Location 4</t>
+  </si>
+  <si>
+    <t>Subject 5</t>
   </si>
   <si>
     <t>6:00</t>
   </si>
   <si>
-    <t>AHOY 5</t>
-  </si>
-  <si>
-    <t>Brazil 5</t>
-  </si>
-  <si>
-    <t>hey 6</t>
+    <t>Description 5</t>
+  </si>
+  <si>
+    <t>Location 5</t>
+  </si>
+  <si>
+    <t>Subject 6</t>
   </si>
   <si>
     <t>7:00</t>
@@ -133,37 +139,37 @@
     <t>TRUE</t>
   </si>
   <si>
-    <t>AHOY 6</t>
-  </si>
-  <si>
-    <t>Brazil 6</t>
-  </si>
-  <si>
-    <t>hey 7</t>
+    <t>Description 6</t>
+  </si>
+  <si>
+    <t>Location 6</t>
+  </si>
+  <si>
+    <t>Subject 7</t>
   </si>
   <si>
     <t>8:00</t>
   </si>
   <si>
-    <t>AHOY 7</t>
-  </si>
-  <si>
-    <t>Brazil 7</t>
-  </si>
-  <si>
-    <t>hey 8</t>
+    <t>Description 7</t>
+  </si>
+  <si>
+    <t>Location 7</t>
+  </si>
+  <si>
+    <t>Subject 8</t>
   </si>
   <si>
     <t>9:00</t>
   </si>
   <si>
-    <t>AHOY 8</t>
-  </si>
-  <si>
-    <t>Brazil 8</t>
-  </si>
-  <si>
-    <t>hey 9</t>
+    <t>Description 8</t>
+  </si>
+  <si>
+    <t>Location 8</t>
+  </si>
+  <si>
+    <t>Subject 9</t>
   </si>
   <si>
     <t>01/27/22</t>
@@ -172,13 +178,13 @@
     <t>10:00</t>
   </si>
   <si>
-    <t>AHOY 9</t>
-  </si>
-  <si>
-    <t>Brazil 9</t>
-  </si>
-  <si>
-    <t>hey 10</t>
+    <t>Description 9</t>
+  </si>
+  <si>
+    <t>Location 9</t>
+  </si>
+  <si>
+    <t>Subject 10</t>
   </si>
   <si>
     <t>01/28/22</t>
@@ -187,433 +193,433 @@
     <t>11:00</t>
   </si>
   <si>
-    <t>AHOY 10</t>
-  </si>
-  <si>
-    <t>Brazil 10</t>
-  </si>
-  <si>
-    <t>hey 11</t>
+    <t>Description 10</t>
+  </si>
+  <si>
+    <t>Location 10</t>
+  </si>
+  <si>
+    <t>Subject 11</t>
   </si>
   <si>
     <t>12:00</t>
   </si>
   <si>
-    <t>AHOY 11</t>
-  </si>
-  <si>
-    <t>Brazil 11</t>
-  </si>
-  <si>
-    <t>hey 12</t>
+    <t>Description 11</t>
+  </si>
+  <si>
+    <t>Location 11</t>
+  </si>
+  <si>
+    <t>Subject 12</t>
   </si>
   <si>
     <t>13:00</t>
   </si>
   <si>
-    <t>AHOY 12</t>
-  </si>
-  <si>
-    <t>Brazil 12</t>
-  </si>
-  <si>
-    <t>hey 13</t>
+    <t>Description 12</t>
+  </si>
+  <si>
+    <t>Location 12</t>
+  </si>
+  <si>
+    <t>Subject 13</t>
   </si>
   <si>
     <t>14:00</t>
   </si>
   <si>
-    <t>AHOY 13</t>
-  </si>
-  <si>
-    <t>Brazil 13</t>
-  </si>
-  <si>
-    <t>hey 14</t>
+    <t>Description 13</t>
+  </si>
+  <si>
+    <t>Location 13</t>
+  </si>
+  <si>
+    <t>Subject 14</t>
   </si>
   <si>
     <t>15:00</t>
   </si>
   <si>
-    <t>AHOY 14</t>
-  </si>
-  <si>
-    <t>Brazil 14</t>
-  </si>
-  <si>
-    <t>hey 15</t>
+    <t>Description 14</t>
+  </si>
+  <si>
+    <t>Location 14</t>
+  </si>
+  <si>
+    <t>Subject 15</t>
   </si>
   <si>
     <t>16:00</t>
   </si>
   <si>
-    <t>AHOY 15</t>
-  </si>
-  <si>
-    <t>Brazil 15</t>
-  </si>
-  <si>
-    <t>hey 16</t>
+    <t>Description 15</t>
+  </si>
+  <si>
+    <t>Location 15</t>
+  </si>
+  <si>
+    <t>Subject 16</t>
   </si>
   <si>
     <t>17:00</t>
   </si>
   <si>
-    <t>AHOY 16</t>
-  </si>
-  <si>
-    <t>Brazil 16</t>
-  </si>
-  <si>
-    <t>hey 17</t>
+    <t>Description 16</t>
+  </si>
+  <si>
+    <t>Location 16</t>
+  </si>
+  <si>
+    <t>Subject 17</t>
   </si>
   <si>
     <t>1:00</t>
   </si>
   <si>
-    <t>AHOY 17</t>
-  </si>
-  <si>
-    <t>Brazil 17</t>
-  </si>
-  <si>
-    <t>hey 18</t>
-  </si>
-  <si>
-    <t>AHOY 18</t>
-  </si>
-  <si>
-    <t>Brazil 18</t>
-  </si>
-  <si>
-    <t>hey 19</t>
-  </si>
-  <si>
-    <t>AHOY 19</t>
-  </si>
-  <si>
-    <t>Brazil 19</t>
-  </si>
-  <si>
-    <t>hey 20</t>
-  </si>
-  <si>
-    <t>AHOY 20</t>
-  </si>
-  <si>
-    <t>Brazil 20</t>
-  </si>
-  <si>
-    <t>hey 21</t>
+    <t>Description 17</t>
+  </si>
+  <si>
+    <t>Location 17</t>
+  </si>
+  <si>
+    <t>Subject 18</t>
+  </si>
+  <si>
+    <t>Description 18</t>
+  </si>
+  <si>
+    <t>Location 18</t>
+  </si>
+  <si>
+    <t>Subject 19</t>
+  </si>
+  <si>
+    <t>Description 19</t>
+  </si>
+  <si>
+    <t>Location 19</t>
+  </si>
+  <si>
+    <t>Subject 20</t>
+  </si>
+  <si>
+    <t>Description 20</t>
+  </si>
+  <si>
+    <t>Location 20</t>
+  </si>
+  <si>
+    <t>Subject 21</t>
   </si>
   <si>
     <t>01/31/22</t>
   </si>
   <si>
-    <t>AHOY 21</t>
-  </si>
-  <si>
-    <t>Brazil 21</t>
-  </si>
-  <si>
-    <t>hey 22</t>
-  </si>
-  <si>
-    <t>AHOY 22</t>
-  </si>
-  <si>
-    <t>Brazil 22</t>
-  </si>
-  <si>
-    <t>hey 23</t>
-  </si>
-  <si>
-    <t>AHOY 23</t>
-  </si>
-  <si>
-    <t>Brazil 23</t>
-  </si>
-  <si>
-    <t>hey 24</t>
-  </si>
-  <si>
-    <t>AHOY 24</t>
-  </si>
-  <si>
-    <t>Brazil 24</t>
-  </si>
-  <si>
-    <t>hey 25</t>
+    <t>Description 21</t>
+  </si>
+  <si>
+    <t>Location 21</t>
+  </si>
+  <si>
+    <t>Subject 22</t>
+  </si>
+  <si>
+    <t>Description 22</t>
+  </si>
+  <si>
+    <t>Location 22</t>
+  </si>
+  <si>
+    <t>Subject 23</t>
+  </si>
+  <si>
+    <t>Description 23</t>
+  </si>
+  <si>
+    <t>Location 23</t>
+  </si>
+  <si>
+    <t>Subject 24</t>
+  </si>
+  <si>
+    <t>Description 24</t>
+  </si>
+  <si>
+    <t>Location 24</t>
+  </si>
+  <si>
+    <t>Subject 25</t>
   </si>
   <si>
     <t>02/03/22</t>
   </si>
   <si>
-    <t>AHOY 25</t>
-  </si>
-  <si>
-    <t>Brazil 25</t>
-  </si>
-  <si>
-    <t>hey 26</t>
-  </si>
-  <si>
-    <t>AHOY 26</t>
-  </si>
-  <si>
-    <t>Brazil 26</t>
-  </si>
-  <si>
-    <t>hey 27</t>
+    <t>Description 25</t>
+  </si>
+  <si>
+    <t>Location 25</t>
+  </si>
+  <si>
+    <t>Subject 26</t>
+  </si>
+  <si>
+    <t>Description 26</t>
+  </si>
+  <si>
+    <t>Location 26</t>
+  </si>
+  <si>
+    <t>Subject 27</t>
   </si>
   <si>
     <t>02/04/22</t>
   </si>
   <si>
-    <t>AHOY 27</t>
-  </si>
-  <si>
-    <t>Brazil 27</t>
-  </si>
-  <si>
-    <t>hey 28</t>
-  </si>
-  <si>
-    <t>AHOY 28</t>
-  </si>
-  <si>
-    <t>Brazil 28</t>
-  </si>
-  <si>
-    <t>hey 29</t>
-  </si>
-  <si>
-    <t>AHOY 29</t>
-  </si>
-  <si>
-    <t>Brazil 29</t>
-  </si>
-  <si>
-    <t>hey 30</t>
-  </si>
-  <si>
-    <t>AHOY 30</t>
-  </si>
-  <si>
-    <t>Brazil 30</t>
-  </si>
-  <si>
-    <t>hey 31</t>
-  </si>
-  <si>
-    <t>AHOY 31</t>
-  </si>
-  <si>
-    <t>Brazil 31</t>
-  </si>
-  <si>
-    <t>hey 32</t>
-  </si>
-  <si>
-    <t>AHOY 32</t>
-  </si>
-  <si>
-    <t>Brazil 32</t>
-  </si>
-  <si>
-    <t>hey 33</t>
+    <t>Description 27</t>
+  </si>
+  <si>
+    <t>Location 27</t>
+  </si>
+  <si>
+    <t>Subject 28</t>
+  </si>
+  <si>
+    <t>Description 28</t>
+  </si>
+  <si>
+    <t>Location 28</t>
+  </si>
+  <si>
+    <t>Subject 29</t>
+  </si>
+  <si>
+    <t>Description 29</t>
+  </si>
+  <si>
+    <t>Location 29</t>
+  </si>
+  <si>
+    <t>Subject 30</t>
+  </si>
+  <si>
+    <t>Description 30</t>
+  </si>
+  <si>
+    <t>Location 30</t>
+  </si>
+  <si>
+    <t>Subject 31</t>
+  </si>
+  <si>
+    <t>Description 31</t>
+  </si>
+  <si>
+    <t>Location 31</t>
+  </si>
+  <si>
+    <t>Subject 32</t>
+  </si>
+  <si>
+    <t>Description 32</t>
+  </si>
+  <si>
+    <t>Location 32</t>
+  </si>
+  <si>
+    <t>Subject 33</t>
   </si>
   <si>
     <t>02/10/22</t>
   </si>
   <si>
-    <t>AHOY 33</t>
-  </si>
-  <si>
-    <t>Brazil 33</t>
-  </si>
-  <si>
-    <t>hey 34</t>
+    <t>Description 33</t>
+  </si>
+  <si>
+    <t>Location 33</t>
+  </si>
+  <si>
+    <t>Subject 34</t>
   </si>
   <si>
     <t>02/11/22</t>
   </si>
   <si>
-    <t>AHOY 34</t>
-  </si>
-  <si>
-    <t>Brazil 34</t>
-  </si>
-  <si>
-    <t>hey 35</t>
-  </si>
-  <si>
-    <t>AHOY 35</t>
-  </si>
-  <si>
-    <t>Brazil 35</t>
-  </si>
-  <si>
-    <t>hey 36</t>
-  </si>
-  <si>
-    <t>AHOY 36</t>
-  </si>
-  <si>
-    <t>Brazil 36</t>
-  </si>
-  <si>
-    <t>hey 37</t>
-  </si>
-  <si>
-    <t>AHOY 37</t>
-  </si>
-  <si>
-    <t>Brazil 37</t>
-  </si>
-  <si>
-    <t>hey 38</t>
-  </si>
-  <si>
-    <t>AHOY 38</t>
-  </si>
-  <si>
-    <t>Brazil 38</t>
-  </si>
-  <si>
-    <t>hey 39</t>
-  </si>
-  <si>
-    <t>AHOY 39</t>
-  </si>
-  <si>
-    <t>Brazil 39</t>
-  </si>
-  <si>
-    <t>hey 40</t>
-  </si>
-  <si>
-    <t>AHOY 40</t>
-  </si>
-  <si>
-    <t>Brazil 40</t>
-  </si>
-  <si>
-    <t>hey 41</t>
-  </si>
-  <si>
-    <t>AHOY 41</t>
-  </si>
-  <si>
-    <t>Brazil 41</t>
-  </si>
-  <si>
-    <t>hey 42</t>
-  </si>
-  <si>
-    <t>AHOY 42</t>
-  </si>
-  <si>
-    <t>Brazil 42</t>
-  </si>
-  <si>
-    <t>hey 43</t>
-  </si>
-  <si>
-    <t>AHOY 43</t>
-  </si>
-  <si>
-    <t>Brazil 43</t>
-  </si>
-  <si>
-    <t>hey 44</t>
-  </si>
-  <si>
-    <t>AHOY 44</t>
-  </si>
-  <si>
-    <t>Brazil 44</t>
-  </si>
-  <si>
-    <t>hey 45</t>
-  </si>
-  <si>
-    <t>AHOY 45</t>
-  </si>
-  <si>
-    <t>Brazil 45</t>
-  </si>
-  <si>
-    <t>hey 46</t>
-  </si>
-  <si>
-    <t>AHOY 46</t>
-  </si>
-  <si>
-    <t>Brazil 46</t>
-  </si>
-  <si>
-    <t>hey 47</t>
+    <t>Description 34</t>
+  </si>
+  <si>
+    <t>Location 34</t>
+  </si>
+  <si>
+    <t>Subject 35</t>
+  </si>
+  <si>
+    <t>Description 35</t>
+  </si>
+  <si>
+    <t>Location 35</t>
+  </si>
+  <si>
+    <t>Subject 36</t>
+  </si>
+  <si>
+    <t>Description 36</t>
+  </si>
+  <si>
+    <t>Location 36</t>
+  </si>
+  <si>
+    <t>Subject 37</t>
+  </si>
+  <si>
+    <t>Description 37</t>
+  </si>
+  <si>
+    <t>Location 37</t>
+  </si>
+  <si>
+    <t>Subject 38</t>
+  </si>
+  <si>
+    <t>Description 38</t>
+  </si>
+  <si>
+    <t>Location 38</t>
+  </si>
+  <si>
+    <t>Subject 39</t>
+  </si>
+  <si>
+    <t>Description 39</t>
+  </si>
+  <si>
+    <t>Location 39</t>
+  </si>
+  <si>
+    <t>Subject 40</t>
+  </si>
+  <si>
+    <t>Description 40</t>
+  </si>
+  <si>
+    <t>Location 40</t>
+  </si>
+  <si>
+    <t>Subject 41</t>
+  </si>
+  <si>
+    <t>Description 41</t>
+  </si>
+  <si>
+    <t>Location 41</t>
+  </si>
+  <si>
+    <t>Subject 42</t>
+  </si>
+  <si>
+    <t>Description 42</t>
+  </si>
+  <si>
+    <t>Location 42</t>
+  </si>
+  <si>
+    <t>Subject 43</t>
+  </si>
+  <si>
+    <t>Description 43</t>
+  </si>
+  <si>
+    <t>Location 43</t>
+  </si>
+  <si>
+    <t>Subject 44</t>
+  </si>
+  <si>
+    <t>Description 44</t>
+  </si>
+  <si>
+    <t>Location 44</t>
+  </si>
+  <si>
+    <t>Subject 45</t>
+  </si>
+  <si>
+    <t>Description 45</t>
+  </si>
+  <si>
+    <t>Location 45</t>
+  </si>
+  <si>
+    <t>Subject 46</t>
+  </si>
+  <si>
+    <t>Description 46</t>
+  </si>
+  <si>
+    <t>Location 46</t>
+  </si>
+  <si>
+    <t>Subject 47</t>
   </si>
   <si>
     <t>02/18/22</t>
   </si>
   <si>
-    <t>AHOY 47</t>
-  </si>
-  <si>
-    <t>Brazil 47</t>
-  </si>
-  <si>
-    <t>hey 48</t>
-  </si>
-  <si>
-    <t>AHOY 48</t>
-  </si>
-  <si>
-    <t>Brazil 48</t>
-  </si>
-  <si>
-    <t>hey 49</t>
+    <t>Description 47</t>
+  </si>
+  <si>
+    <t>Location 47</t>
+  </si>
+  <si>
+    <t>Subject 48</t>
+  </si>
+  <si>
+    <t>Description 48</t>
+  </si>
+  <si>
+    <t>Location 48</t>
+  </si>
+  <si>
+    <t>Subject 49</t>
   </si>
   <si>
     <t>03/08/22</t>
   </si>
   <si>
-    <t>AHOY 49</t>
-  </si>
-  <si>
-    <t>Brazil 49</t>
-  </si>
-  <si>
-    <t>hey 50</t>
-  </si>
-  <si>
-    <t>AHOY 50</t>
-  </si>
-  <si>
-    <t>Brazil 50</t>
-  </si>
-  <si>
-    <t>hey 51</t>
+    <t>Description 49</t>
+  </si>
+  <si>
+    <t>Location 49</t>
+  </si>
+  <si>
+    <t>Subject 50</t>
+  </si>
+  <si>
+    <t>Description 50</t>
+  </si>
+  <si>
+    <t>Location 50</t>
+  </si>
+  <si>
+    <t>Subject 51</t>
   </si>
   <si>
     <t>03/22/22</t>
   </si>
   <si>
-    <t>AHOY 51</t>
-  </si>
-  <si>
-    <t>Brazil 51</t>
-  </si>
-  <si>
-    <t>hey 52</t>
-  </si>
-  <si>
-    <t>AHOY 52</t>
-  </si>
-  <si>
-    <t>Brazil 52</t>
+    <t>Description 51</t>
+  </si>
+  <si>
+    <t>Location 51</t>
+  </si>
+  <si>
+    <t>Subject 52</t>
+  </si>
+  <si>
+    <t>Description 52</t>
+  </si>
+  <si>
+    <t>Location 52</t>
   </si>
 </sst>
 </file>
@@ -959,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G53"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1020,1486 +1026,1486 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I17" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I19" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I20" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G21" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H21" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I21" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H22" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I23" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E24" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G24" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H24" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I24" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H25" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I25" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D26" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E26" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H26" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I26" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H27" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I27" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H28" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G29" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H29" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I29" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D30" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E30" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H30" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I30" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E31" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H31" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I31" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H32" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I32" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D33" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G33" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H33" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G34" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H34" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I34" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G35" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H35" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I35" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G36" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H36" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I36" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F37" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H37" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I37" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E38" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H38" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I38" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E39" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G39" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H39" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I39" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E40" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H40" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="I40" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E41" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H41" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="I41" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E42" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F42" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G42" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H42" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I42" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C43" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D43" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E43" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G43" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H43" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I43" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D44" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E44" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F44" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G44" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H44" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="I44" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E45" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G45" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H45" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="I45" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C46" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D46" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E46" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F46" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G46" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H46" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I46" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C47" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E47" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F47" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H47" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="I47" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C48" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D48" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E48" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F48" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G48" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H48" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="I48" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C49" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D49" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E49" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F49" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G49" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H49" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="I49" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C50" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D50" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E50" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F50" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G50" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H50" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I50" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C51" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D51" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E51" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="G51" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H51" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="I51" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C52" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D52" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E52" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F52" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="G52" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H52" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I52" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C53" t="s">
         <v>11</v>
       </c>
       <c r="D53" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E53" t="s">
         <v>11</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="G53" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H53" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="I53" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>